<commit_message>
this commit on 22 may by pradyumna
</commit_message>
<xml_diff>
--- a/crypto.xlsx
+++ b/crypto.xlsx
@@ -515,25 +515,25 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>19377631</v>
+        <v>19380193</v>
       </c>
       <c r="F2" t="n">
         <v>21000000</v>
       </c>
       <c r="G2" t="n">
-        <v>520916218620.9102</v>
+        <v>520574764926.9825</v>
       </c>
       <c r="H2" t="n">
-        <v>3952258752.122029</v>
+        <v>2597289392.164969</v>
       </c>
       <c r="I2" t="n">
-        <v>26882.34793101954</v>
+        <v>26861.17547575417</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.805624507337366</v>
+        <v>-0.8223954943998436</v>
       </c>
       <c r="K2" t="n">
-        <v>26929.83849322836</v>
+        <v>26855.6945808924</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -561,23 +561,23 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>120275672.4515426</v>
+        <v>120269409.4694304</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
-        <v>217658200063.3058</v>
+        <v>218004078163.9951</v>
       </c>
       <c r="H3" t="n">
-        <v>2295052616.975626</v>
+        <v>1467512592.037269</v>
       </c>
       <c r="I3" t="n">
-        <v>1809.661053036285</v>
+        <v>1812.631151393542</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.031194738982729</v>
+        <v>-0.2507876472408797</v>
       </c>
       <c r="K3" t="n">
-        <v>1805.408492149117</v>
+        <v>1807.826990018449</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -605,23 +605,23 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>82856924178.67105</v>
+        <v>82919078535.20427</v>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
-        <v>82866794017.61983</v>
+        <v>82903163875.13692</v>
       </c>
       <c r="H4" t="n">
-        <v>7026431365.335028</v>
+        <v>4562518091.345233</v>
       </c>
       <c r="I4" t="n">
-        <v>1.000119119060315</v>
+        <v>0.9998080699840316</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0169127313098004</v>
+        <v>-0.0408501284214867</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9994514873252784</v>
+        <v>0.9994026091884856</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -655,19 +655,19 @@
         <v>166801148</v>
       </c>
       <c r="G5" t="n">
-        <v>51701581863.25945</v>
+        <v>51213417817.62611</v>
       </c>
       <c r="H5" t="n">
-        <v>140146567.1523465</v>
+        <v>94428505.71872495</v>
       </c>
       <c r="I5" t="n">
-        <v>309.9593886683529</v>
+        <v>307.0327658513843</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.973895360107543</v>
+        <v>-1.259055227135489</v>
       </c>
       <c r="K5" t="n">
-        <v>310.2842998324977</v>
+        <v>308.3264677003265</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -695,23 +695,23 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>29589576999.19225</v>
+        <v>29547985786.96285</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>29590150139.76532</v>
+        <v>29539423998.57761</v>
       </c>
       <c r="H6" t="n">
-        <v>465210096.8144696</v>
+        <v>309705942.4291187</v>
       </c>
       <c r="I6" t="n">
-        <v>1.000019369677812</v>
+        <v>0.9997102412175582</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.004029418635371</v>
+        <v>-0.0463177930573528</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9999170671063676</v>
+        <v>0.9997664373708528</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -745,19 +745,19 @@
         <v>100000000000</v>
       </c>
       <c r="G7" t="n">
-        <v>21038944244.2304</v>
+        <v>21049341885.85394</v>
       </c>
       <c r="H7" t="n">
-        <v>530334965.8953091</v>
+        <v>283626788.6252815</v>
       </c>
       <c r="I7" t="n">
-        <v>0.4633717507986841</v>
+        <v>0.4636007534210283</v>
       </c>
       <c r="J7" t="n">
-        <v>3.936992077699494</v>
+        <v>-1.285329815687895</v>
       </c>
       <c r="K7" t="n">
-        <v>0.4621680021181822</v>
+        <v>0.4600959050564299</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -785,25 +785,25 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>34858598077.147</v>
+        <v>34863137663.585</v>
       </c>
       <c r="F8" t="n">
         <v>45000000000</v>
       </c>
       <c r="G8" t="n">
-        <v>12917467101.18224</v>
+        <v>12692441935.3907</v>
       </c>
       <c r="H8" t="n">
-        <v>74016601.65892321</v>
+        <v>46282991.71158508</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3705676020760806</v>
+        <v>0.364064819921476</v>
       </c>
       <c r="J8" t="n">
-        <v>-1.72198838451532</v>
+        <v>-0.3261701063882446</v>
       </c>
       <c r="K8" t="n">
-        <v>0.3729860084756148</v>
+        <v>0.3612738943236675</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -831,23 +831,23 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>139407296383.7052</v>
+        <v>139445906383.7052</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>10257489580.04649</v>
+        <v>10029562784.16424</v>
       </c>
       <c r="H9" t="n">
-        <v>123169948.3687851</v>
+        <v>72786045.74362074</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0735792877857249</v>
+        <v>0.0719243973829284</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.6862488531595009</v>
+        <v>-2.559510977439898</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0735363059111897</v>
+        <v>0.0723413235015682</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -881,19 +881,19 @@
         <v>10000000000</v>
       </c>
       <c r="G10" t="n">
-        <v>8117963708.498319</v>
+        <v>7937866808.059611</v>
       </c>
       <c r="H10" t="n">
-        <v>108874049.2957507</v>
+        <v>53247726.80537405</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8748306231623535</v>
+        <v>0.8554225191971353</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.3883316442407272</v>
+        <v>-2.331589440572046</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8676338333347891</v>
+        <v>0.8612912883302764</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -921,23 +921,23 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>395774597.4627099</v>
+        <v>396087768.0440765</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
-        <v>8098088629.382645</v>
+        <v>7823086788.890805</v>
       </c>
       <c r="H11" t="n">
-        <v>70957568.46508439</v>
+        <v>77492852.29093248</v>
       </c>
       <c r="I11" t="n">
-        <v>20.46136533597423</v>
+        <v>19.75089215080294</v>
       </c>
       <c r="J11" t="n">
-        <v>-1.958823994770285</v>
+        <v>-2.460182917513592</v>
       </c>
       <c r="K11" t="n">
-        <v>20.48533807744683</v>
+        <v>19.80297360247333</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -948,7 +948,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>litecoin</t>
+          <t>tron</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -956,45 +956,43 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>72952601.80932352</v>
-      </c>
-      <c r="F12" t="n">
-        <v>84000000</v>
-      </c>
+        <v>90346655403.25447</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>6706776648.140532</v>
+        <v>6765867014.919566</v>
       </c>
       <c r="H12" t="n">
-        <v>260450939.7747888</v>
+        <v>117076628.9331392</v>
       </c>
       <c r="I12" t="n">
-        <v>91.93334414131053</v>
+        <v>0.0748878526241033</v>
       </c>
       <c r="J12" t="n">
-        <v>-1.113710468663544</v>
+        <v>3.337457470437678</v>
       </c>
       <c r="K12" t="n">
-        <v>91.50395462499232</v>
+        <v>0.0749009845752413</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>http://explorer.litecoin.net/chain/Litecoin</t>
+          <t>https://tronscan.org/#/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>polkadot</t>
+          <t>litecoin</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1002,43 +1000,45 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1233748488.22675</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
+        <v>72973939.30932352</v>
+      </c>
+      <c r="F13" t="n">
+        <v>84000000</v>
+      </c>
       <c r="G13" t="n">
-        <v>6608611689.142522</v>
+        <v>6665607211.235456</v>
       </c>
       <c r="H13" t="n">
-        <v>41805299.4289281</v>
+        <v>182817775.1072488</v>
       </c>
       <c r="I13" t="n">
-        <v>5.356530729079952</v>
+        <v>91.34229663799751</v>
       </c>
       <c r="J13" t="n">
-        <v>-1.401432648692291</v>
+        <v>-0.9993837594520296</v>
       </c>
       <c r="K13" t="n">
-        <v>5.358024114918685</v>
+        <v>91.97618873684</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>https://polkascan.io/polkadot</t>
+          <t>http://explorer.litecoin.net/chain/Litecoin</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>tron</t>
+          <t>polkadot</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1046,36 +1046,36 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>90376479958.22383</v>
+        <v>1234641350.23399</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>6372361430.768843</v>
+        <v>6548341675.583468</v>
       </c>
       <c r="H14" t="n">
-        <v>47086418.92241599</v>
+        <v>40982892.79630226</v>
       </c>
       <c r="I14" t="n">
-        <v>0.070509068661608</v>
+        <v>5.303841212140208</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.08096135824848839</v>
+        <v>-1.645266069168453</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0705984551728195</v>
+        <v>5.301615134041474</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>https://tronscan.org/#/</t>
+          <t>https://polkascan.io/polkadot</t>
         </is>
       </c>
     </row>
@@ -1099,23 +1099,23 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>5544850540.053376</v>
+        <v>5499801594.053376</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>5546014716.200308</v>
+        <v>5497735372.429612</v>
       </c>
       <c r="H15" t="n">
-        <v>195939323.4133282</v>
+        <v>100221171.3488173</v>
       </c>
       <c r="I15" t="n">
-        <v>1.000209956271774</v>
+        <v>0.999624309788557</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.0067319489556465</v>
+        <v>-0.0306253404030405</v>
       </c>
       <c r="K15" t="n">
-        <v>0.9999507392654896</v>
+        <v>0.9999576623305436</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
@@ -1147,19 +1147,19 @@
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
-        <v>5123619759.012672</v>
+        <v>5062227729.736824</v>
       </c>
       <c r="H16" t="n">
-        <v>38162179.04488184</v>
+        <v>34312729.07316222</v>
       </c>
       <c r="I16" t="n">
-        <v>8.690960758799999e-06</v>
+        <v>8.586824280600001e-06</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.360245522112362</v>
+        <v>-1.315316788457194</v>
       </c>
       <c r="K16" t="n">
-        <v>8.693421789700001e-06</v>
+        <v>8.567503069999999e-06</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
@@ -1170,7 +1170,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>avalanche</t>
+          <t>multi-collateral-dai</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1178,45 +1178,43 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Multi Collateral DAI</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>333513819.7964773</v>
-      </c>
-      <c r="F17" t="n">
-        <v>720000000</v>
-      </c>
+        <v>4854516237.35908</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
-        <v>4911993405.754802</v>
+        <v>4857620055.61681</v>
       </c>
       <c r="H17" t="n">
-        <v>35912250.23763216</v>
+        <v>14141878.52468326</v>
       </c>
       <c r="I17" t="n">
-        <v>14.7280056003445</v>
+        <v>1.000639367159562</v>
       </c>
       <c r="J17" t="n">
-        <v>-2.415563738150442</v>
+        <v>-0.0790074327931638</v>
       </c>
       <c r="K17" t="n">
-        <v>14.74177697658721</v>
+        <v>1.000454175818275</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>https://avascan.info/</t>
+          <t>https://etherscan.io/token/0x89d24a6b4ccb1b6faa2625fe562bdd9a23260359</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>multi-collateral-dai</t>
+          <t>avalanche</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1224,36 +1222,38 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Multi Collateral DAI</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>4865713842.042386</v>
-      </c>
-      <c r="F18" t="inlineStr"/>
+        <v>334137203.2993836</v>
+      </c>
+      <c r="F18" t="n">
+        <v>720000000</v>
+      </c>
       <c r="G18" t="n">
-        <v>4866954874.708639</v>
+        <v>4811074581.48767</v>
       </c>
       <c r="H18" t="n">
-        <v>24945996.20692766</v>
+        <v>28549774.48598316</v>
       </c>
       <c r="I18" t="n">
-        <v>1.000255056648735</v>
+        <v>14.39850017891302</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.009645280005001901</v>
+        <v>-1.600087125828313</v>
       </c>
       <c r="K18" t="n">
-        <v>1.001316070565994</v>
+        <v>14.36067327813482</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x89d24a6b4ccb1b6faa2625fe562bdd9a23260359</t>
+          <t>https://avascan.info/</t>
         </is>
       </c>
     </row>
@@ -1277,23 +1277,23 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>155059.29266951</v>
+        <v>155648.58481214</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
-        <v>4171916679.064941</v>
+        <v>4186037054.882479</v>
       </c>
       <c r="H19" t="n">
-        <v>37314239.17349496</v>
+        <v>25408077.69909868</v>
       </c>
       <c r="I19" t="n">
-        <v>26905.29930351787</v>
+        <v>26894.1542895158</v>
       </c>
       <c r="J19" t="n">
-        <v>-1.770811786008448</v>
+        <v>-0.8066177098348529</v>
       </c>
       <c r="K19" t="n">
-        <v>26923.08791895764</v>
+        <v>26849.45899018364</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1327,19 +1327,19 @@
         <v>1000000000</v>
       </c>
       <c r="G20" t="n">
-        <v>3362138496.757148</v>
+        <v>3345090041.824169</v>
       </c>
       <c r="H20" t="n">
-        <v>65707044.46754844</v>
+        <v>50796587.45678969</v>
       </c>
       <c r="I20" t="n">
-        <v>6.501911987759676</v>
+        <v>6.468942628047568</v>
       </c>
       <c r="J20" t="n">
-        <v>-3.221470953997284</v>
+        <v>-0.7052931258228063</v>
       </c>
       <c r="K20" t="n">
-        <v>6.562147620067249</v>
+        <v>6.434389588546103</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -1350,7 +1350,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>uniswap</t>
+          <t>unus-sed-leo</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1358,45 +1358,43 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>UNUS SED LEO</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>577501036</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1000000000</v>
-      </c>
+        <v>930314421.9</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>3067254493.502509</v>
+        <v>3308970810.08931</v>
       </c>
       <c r="H21" t="n">
-        <v>15283007.20301714</v>
+        <v>248246.5166598</v>
       </c>
       <c r="I21" t="n">
-        <v>5.311253664144957</v>
+        <v>3.556830607152506</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.8362286201368395</v>
+        <v>-1.865821175457968</v>
       </c>
       <c r="K21" t="n">
-        <v>5.293323668936263</v>
+        <v>3.571330371960817</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x1f9840a85d5af5bf1d1762f925bdaddc4201f984</t>
+          <t>https://eospark.com/account/bitfinexleo1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>monero</t>
+          <t>uniswap</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1404,43 +1402,45 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>18280679.37319591</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
+        <v>577501036</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1000000000</v>
+      </c>
       <c r="G22" t="n">
-        <v>2769531136.930362</v>
+        <v>2951544236.962595</v>
       </c>
       <c r="H22" t="n">
-        <v>31878040.8491924</v>
+        <v>14306379.98432856</v>
       </c>
       <c r="I22" t="n">
-        <v>151.500449211488</v>
+        <v>5.110889942996732</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2061070423808614</v>
+        <v>-2.57293116054122</v>
       </c>
       <c r="K22" t="n">
-        <v>151.0118406921045</v>
+        <v>5.152041056605529</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>http://moneroblocks.info/</t>
+          <t>https://etherscan.io/token/0x1f9840a85d5af5bf1d1762f925bdaddc4201f984</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>okb</t>
+          <t>monero</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1448,36 +1448,36 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>60000000</v>
+        <v>18281909.36057431</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>2734320721.88663</v>
+        <v>2749365660.007049</v>
       </c>
       <c r="H23" t="n">
-        <v>207136.939871046</v>
+        <v>21975076.47839453</v>
       </c>
       <c r="I23" t="n">
-        <v>45.57201203144383</v>
+        <v>150.3872273831621</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.6310815061001457</v>
+        <v>-0.0564336239958503</v>
       </c>
       <c r="K23" t="n">
-        <v>45.76813483145782</v>
+        <v>150.2071555978359</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x75231f58b43240c9718dd58b4967c5114342a86c</t>
+          <t>http://moneroblocks.info/</t>
         </is>
       </c>
     </row>
@@ -1505,19 +1505,19 @@
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
-        <v>2634635201.514927</v>
+        <v>2600898541.056958</v>
       </c>
       <c r="H24" t="n">
-        <v>43533644.9992281</v>
+        <v>24902296.80229991</v>
       </c>
       <c r="I24" t="n">
-        <v>10.60415076525791</v>
+        <v>10.46836398399616</v>
       </c>
       <c r="J24" t="n">
-        <v>-3.058009603759801</v>
+        <v>-0.9105376199009486</v>
       </c>
       <c r="K24" t="n">
-        <v>10.752809395012</v>
+        <v>10.48193365905663</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
@@ -1545,25 +1545,25 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>141011721.2409984</v>
+        <v>141058463.1549442</v>
       </c>
       <c r="F25" t="n">
         <v>210700000</v>
       </c>
       <c r="G25" t="n">
-        <v>2585854518.856635</v>
+        <v>2541935119.473046</v>
       </c>
       <c r="H25" t="n">
-        <v>33654806.63719088</v>
+        <v>28049969.86415119</v>
       </c>
       <c r="I25" t="n">
-        <v>18.3378693352536</v>
+        <v>18.02043679350798</v>
       </c>
       <c r="J25" t="n">
-        <v>-1.349589940951608</v>
+        <v>-1.7812331008022</v>
       </c>
       <c r="K25" t="n">
-        <v>18.34632330400821</v>
+        <v>18.06858631109104</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
@@ -1591,25 +1591,25 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>26778812338.17499</v>
+        <v>26793793987.20616</v>
       </c>
       <c r="F26" t="n">
         <v>50001806812</v>
       </c>
       <c r="G26" t="n">
-        <v>2383324077.747151</v>
+        <v>2364893900.020615</v>
       </c>
       <c r="H26" t="n">
-        <v>13639590.88977488</v>
+        <v>9900029.7013181</v>
       </c>
       <c r="I26" t="n">
-        <v>0.08900036520101989</v>
+        <v>0.08826274849876931</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.0783137578573579</v>
+        <v>-1.18025835173709</v>
       </c>
       <c r="K26" t="n">
-        <v>0.08893232864262229</v>
+        <v>0.08838024027936291</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
@@ -1620,7 +1620,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>internet-computer</t>
+          <t>bitcoin-cash</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1628,43 +1628,45 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>436286672.5692753</v>
-      </c>
-      <c r="F27" t="inlineStr"/>
+        <v>19398287.5</v>
+      </c>
+      <c r="F27" t="n">
+        <v>21000000</v>
+      </c>
       <c r="G27" t="n">
-        <v>2325180583.766084</v>
+        <v>2224450404.805701</v>
       </c>
       <c r="H27" t="n">
-        <v>9276857.984196611</v>
+        <v>11964680.30325451</v>
       </c>
       <c r="I27" t="n">
-        <v>5.329478826554993</v>
+        <v>114.6725145096288</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.4438979869280933</v>
+        <v>-1.57469031449445</v>
       </c>
       <c r="K27" t="n">
-        <v>5.272056519387822</v>
+        <v>114.917294663821</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>https://www.dfinityexplorer.org/#/</t>
+          <t>https://blockchair.com/bitcoin-cash/blocks</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>bitcoin-cash</t>
+          <t>internet-computer</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1672,38 +1674,36 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>19395681.25</v>
-      </c>
-      <c r="F28" t="n">
-        <v>21000000</v>
-      </c>
+        <v>436311135.2514898</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="n">
-        <v>2244888290.815117</v>
+        <v>2217205600.398755</v>
       </c>
       <c r="H28" t="n">
-        <v>20710580.49027814</v>
+        <v>8457940.691628413</v>
       </c>
       <c r="I28" t="n">
-        <v>115.7416572215073</v>
+        <v>5.081707573474505</v>
       </c>
       <c r="J28" t="n">
-        <v>-1.232499554779439</v>
+        <v>-2.186569242285849</v>
       </c>
       <c r="K28" t="n">
-        <v>115.6592931745815</v>
+        <v>5.069318783724567</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>https://blockchair.com/bitcoin-cash/blocks</t>
+          <t>https://www.dfinityexplorer.org/#/</t>
         </is>
       </c>
     </row>
@@ -1727,23 +1727,23 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>2083944076.54</v>
+        <v>2081362134.18</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>2083367393.553021</v>
+        <v>2079111507.255876</v>
       </c>
       <c r="H29" t="n">
-        <v>156189689.2015267</v>
+        <v>92782320.97688423</v>
       </c>
       <c r="I29" t="n">
-        <v>0.9997232732905502</v>
+        <v>0.9989186759539996</v>
       </c>
       <c r="J29" t="n">
-        <v>0.0383880519598896</v>
+        <v>-0.0583161828162955</v>
       </c>
       <c r="K29" t="n">
-        <v>0.99972495306797</v>
+        <v>0.999586632897248</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
@@ -1771,23 +1771,23 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>425813269</v>
+        <v>426073442</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
-        <v>1897469175.350074</v>
+        <v>1870209171.938469</v>
       </c>
       <c r="H30" t="n">
-        <v>34501525.48145981</v>
+        <v>25299177.2991515</v>
       </c>
       <c r="I30" t="n">
-        <v>4.456106264152313</v>
+        <v>4.389405646030549</v>
       </c>
       <c r="J30" t="n">
-        <v>-2.265488758235781</v>
+        <v>-2.495592253657821</v>
       </c>
       <c r="K30" t="n">
-        <v>4.47739477787205</v>
+        <v>4.403700306677324</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
@@ -1815,25 +1815,25 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>879296562.4172237</v>
+        <v>879304328.0334899</v>
       </c>
       <c r="F31" t="n">
         <v>1000000000</v>
       </c>
       <c r="G31" t="n">
-        <v>1889990683.097461</v>
+        <v>1804839457.345575</v>
       </c>
       <c r="H31" t="n">
-        <v>9909268.984856227</v>
+        <v>2466305.35354314</v>
       </c>
       <c r="I31" t="n">
-        <v>2.149434859499275</v>
+        <v>2.052576565137565</v>
       </c>
       <c r="J31" t="n">
-        <v>-6.118272281071062</v>
+        <v>-3.032573065497764</v>
       </c>
       <c r="K31" t="n">
-        <v>2.194221192279982</v>
+        <v>2.078750878088264</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
@@ -1867,19 +1867,19 @@
         <v>30263013692</v>
       </c>
       <c r="G32" t="n">
-        <v>1583855565.221727</v>
+        <v>1566181944.058229</v>
       </c>
       <c r="H32" t="n">
-        <v>2473763.675987819</v>
+        <v>1700562.294738423</v>
       </c>
       <c r="I32" t="n">
-        <v>0.0626946406526029</v>
+        <v>0.0619950558216334</v>
       </c>
       <c r="J32" t="n">
-        <v>-1.593253996594731</v>
+        <v>-0.1309004141016882</v>
       </c>
       <c r="K32" t="n">
-        <v>0.06272407864092309</v>
+        <v>0.0620284929844319</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
@@ -1907,23 +1907,23 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>906505224</v>
+        <v>907621343</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
-        <v>1511870793.767708</v>
+        <v>1462269319.51655</v>
       </c>
       <c r="H33" t="n">
-        <v>23568582.54252001</v>
+        <v>20820006.05590158</v>
       </c>
       <c r="I33" t="n">
-        <v>1.667801523632156</v>
+        <v>1.611100632212161</v>
       </c>
       <c r="J33" t="n">
-        <v>-1.168404945346741</v>
+        <v>-2.601730589745903</v>
       </c>
       <c r="K33" t="n">
-        <v>1.66289870896829</v>
+        <v>1.617681320147908</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
@@ -1951,23 +1951,23 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>53802.526531</v>
+        <v>53802.81167638</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>1445778660.652939</v>
+        <v>1445067444.089531</v>
       </c>
       <c r="H34" t="n">
-        <v>175766555.4514302</v>
+        <v>105905356.948921</v>
       </c>
       <c r="I34" t="n">
-        <v>26871.94735771208</v>
+        <v>26858.58599326568</v>
       </c>
       <c r="J34" t="n">
-        <v>-1.835240612673658</v>
+        <v>-0.8409494253857482</v>
       </c>
       <c r="K34" t="n">
-        <v>26926.19447654692</v>
+        <v>26827.49245114658</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
@@ -2001,19 +2001,19 @@
         <v>86712634466</v>
       </c>
       <c r="G35" t="n">
-        <v>1431053602.719233</v>
+        <v>1387394266.613124</v>
       </c>
       <c r="H35" t="n">
-        <v>11747269.23609527</v>
+        <v>9702197.338243628</v>
       </c>
       <c r="I35" t="n">
-        <v>0.0196804388590821</v>
+        <v>0.0190800176776311</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.5584763935341236</v>
+        <v>-1.342679529662081</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0195427990613399</v>
+        <v>0.0190346389036247</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
@@ -2047,19 +2047,19 @@
         <v>14881364</v>
       </c>
       <c r="G36" t="n">
-        <v>1253756236.887715</v>
+        <v>1235789785.200922</v>
       </c>
       <c r="H36" t="n">
-        <v>10412951.17637107</v>
+        <v>4038826.185564989</v>
       </c>
       <c r="I36" t="n">
-        <v>103.850198429529</v>
+        <v>102.3620147476837</v>
       </c>
       <c r="J36" t="n">
-        <v>-1.414449787213985</v>
+        <v>-1.508491133441616</v>
       </c>
       <c r="K36" t="n">
-        <v>104.3100166915304</v>
+        <v>102.6022917908294</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
@@ -2087,25 +2087,25 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>7227970188.262621</v>
+        <v>7240768442.795022</v>
       </c>
       <c r="F37" t="n">
         <v>10000000000</v>
       </c>
       <c r="G37" t="n">
-        <v>1202514119.777923</v>
+        <v>1173090903.936224</v>
       </c>
       <c r="H37" t="n">
-        <v>18803744.30892529</v>
+        <v>13476178.29729495</v>
       </c>
       <c r="I37" t="n">
-        <v>0.1663695461459796</v>
+        <v>0.1620119346729719</v>
       </c>
       <c r="J37" t="n">
-        <v>-2.416784961185729</v>
+        <v>-1.352081071247731</v>
       </c>
       <c r="K37" t="n">
-        <v>0.1665677659976466</v>
+        <v>0.1618303827382369</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
@@ -2133,23 +2133,23 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>8986612178.560974</v>
+        <v>8987868251.070761</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="n">
-        <v>1105253446.752345</v>
+        <v>1069790690.120072</v>
       </c>
       <c r="H38" t="n">
-        <v>12750192.97807467</v>
+        <v>8662906.16689218</v>
       </c>
       <c r="I38" t="n">
-        <v>0.1229888888928697</v>
+        <v>0.1190260760656592</v>
       </c>
       <c r="J38" t="n">
-        <v>-0.6257094080794416</v>
+        <v>-1.582491743940783</v>
       </c>
       <c r="K38" t="n">
-        <v>0.1218508587479616</v>
+        <v>0.1187441588931195</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
@@ -2160,7 +2160,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>paxos-standard</t>
+          <t>fantom</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -2168,41 +2168,45 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>USDP</t>
+          <t>FTM</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Pax Dollar</t>
+          <t>Fantom</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1043561366.810683</v>
-      </c>
-      <c r="F39" t="inlineStr"/>
+        <v>2788599947.791616</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3175000000</v>
+      </c>
       <c r="G39" t="n">
-        <v>1043144613.387728</v>
+        <v>1004960152.739064</v>
       </c>
       <c r="H39" t="n">
-        <v>28052678.56815797</v>
+        <v>24710357.06598627</v>
       </c>
       <c r="I39" t="n">
-        <v>0.9996006431090591</v>
+        <v>0.3603816149874508</v>
       </c>
       <c r="J39" t="n">
-        <v>0.0227046904951943</v>
-      </c>
-      <c r="K39" t="inlineStr"/>
+        <v>-3.094435736947408</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.3636902831183378</v>
+      </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x8e870d67f660d95d5be530380d0ec0bd388289e1</t>
+          <t>https://etherscan.io/token/0x4e15361fd6b4bb609fa63c81a2be19d873717870</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>fantom</t>
+          <t>rocket-pool</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -2210,45 +2214,43 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>FTM</t>
+          <t>RPL</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Fantom</t>
+          <t>Rocket Pool</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2788577045.022473</v>
-      </c>
-      <c r="F40" t="n">
-        <v>3175000000</v>
-      </c>
+        <v>19401717.08844526</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="n">
-        <v>1036063817.288923</v>
+        <v>978236587.2863506</v>
       </c>
       <c r="H40" t="n">
-        <v>43331199.42368249</v>
+        <v>396133.4798841552</v>
       </c>
       <c r="I40" t="n">
-        <v>0.3715385304265721</v>
+        <v>50.4201036860259</v>
       </c>
       <c r="J40" t="n">
-        <v>-3.528147224453321</v>
+        <v>0.2756205676510651</v>
       </c>
       <c r="K40" t="n">
-        <v>0.3743371969946109</v>
+        <v>49.76169093759786</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x4e15361fd6b4bb609fa63c81a2be19d873717870</t>
+          <t>https://etherscan.io/token/0xb4efd85c19999d84251304bda99e90b92300bd93</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>frax</t>
+          <t>the-sandbox</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -2256,43 +2258,45 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>SAND</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>The Sandbox</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>1004141409.408784</v>
-      </c>
-      <c r="F41" t="inlineStr"/>
+        <v>1853581926.223322</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3000000000</v>
+      </c>
       <c r="G41" t="n">
-        <v>1003835303.954471</v>
+        <v>949842245.5623848</v>
       </c>
       <c r="H41" t="n">
-        <v>2477285.817876226</v>
+        <v>13141321.83480055</v>
       </c>
       <c r="I41" t="n">
-        <v>0.9996951570252508</v>
+        <v>0.5124360742433924</v>
       </c>
       <c r="J41" t="n">
-        <v>0.0073632469667021</v>
+        <v>-2.490348432622775</v>
       </c>
       <c r="K41" t="n">
-        <v>0.9930516389754704</v>
+        <v>0.5143558230623722</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x853d955acef822db058eb8505911ed77f175b99e</t>
+          <t>https://etherscan.io/token/0x3845badAde8e6dFF049820680d1F14bD3903a5d0</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>the-sandbox</t>
+          <t>eos</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -2300,45 +2304,43 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SAND</t>
+          <t>EOS</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>The Sandbox</t>
+          <t>EOS</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>1853581926.223322</v>
-      </c>
-      <c r="F42" t="n">
-        <v>3000000000</v>
-      </c>
+        <v>1091728054.7351</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
       <c r="G42" t="n">
-        <v>985301607.7722285</v>
+        <v>933970381.0472205</v>
       </c>
       <c r="H42" t="n">
-        <v>23678928.91267502</v>
+        <v>33116570.35154357</v>
       </c>
       <c r="I42" t="n">
-        <v>0.5315662576510889</v>
+        <v>0.8554972797450383</v>
       </c>
       <c r="J42" t="n">
-        <v>-0.3449761729820241</v>
+        <v>-2.647066444060981</v>
       </c>
       <c r="K42" t="n">
-        <v>0.5288350868742944</v>
+        <v>0.8591550927580531</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x3845badAde8e6dFF049820680d1F14bD3903a5d0</t>
+          <t>https://bloks.io/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>eos</t>
+          <t>aave</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -2346,43 +2348,45 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>EOS</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>EOS</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>1091460804.8609</v>
-      </c>
-      <c r="F43" t="inlineStr"/>
+        <v>14396401.17325285</v>
+      </c>
+      <c r="F43" t="n">
+        <v>16000000</v>
+      </c>
       <c r="G43" t="n">
-        <v>971608654.9409306</v>
+        <v>915413504.8454996</v>
       </c>
       <c r="H43" t="n">
-        <v>29950139.30882326</v>
+        <v>10549591.2655429</v>
       </c>
       <c r="I43" t="n">
-        <v>0.8901910637686675</v>
+        <v>63.58627366860624</v>
       </c>
       <c r="J43" t="n">
-        <v>-1.710348822847247</v>
+        <v>-1.984740112710119</v>
       </c>
       <c r="K43" t="n">
-        <v>0.8909060365816712</v>
+        <v>64.03571281520736</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>https://bloks.io/</t>
+          <t>https://etherscan.io/token/0x80fB784B7eD66730e8b1DBd9820aFD29931aab03</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>rocket-pool</t>
+          <t>decentraland</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2390,43 +2394,43 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>RPL</t>
+          <t>MANA</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Rocket Pool</t>
+          <t>Decentraland</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>19401717.08844526</v>
+        <v>1878271531.829944</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
-        <v>965963145.55683</v>
+        <v>898538541.1359886</v>
       </c>
       <c r="H44" t="n">
-        <v>1121994.74646845</v>
+        <v>12486022.61260329</v>
       </c>
       <c r="I44" t="n">
-        <v>49.78750804134298</v>
+        <v>0.478385859503801</v>
       </c>
       <c r="J44" t="n">
-        <v>-1.113887791184755</v>
+        <v>-1.570408646516852</v>
       </c>
       <c r="K44" t="n">
-        <v>49.67198104561687</v>
+        <v>0.4807711075029902</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xb4efd85c19999d84251304bda99e90b92300bd93</t>
+          <t>https://etherscan.io/token/decentraland</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>decentraland</t>
+          <t>kava</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -2434,43 +2438,43 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MANA</t>
+          <t>KAVA</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Decentraland</t>
+          <t>Kava</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1878271531.829944</v>
+        <v>529677522</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="n">
-        <v>935917158.1385164</v>
+        <v>896911146.0479354</v>
       </c>
       <c r="H45" t="n">
-        <v>20596415.23882638</v>
+        <v>21285168.80684207</v>
       </c>
       <c r="I45" t="n">
-        <v>0.4982863991058206</v>
+        <v>1.693315477427293</v>
       </c>
       <c r="J45" t="n">
-        <v>-1.791569567853405</v>
+        <v>-2.221821121698776</v>
       </c>
       <c r="K45" t="n">
-        <v>0.5021062631373784</v>
+        <v>1.220717982863031</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/decentraland</t>
+          <t>https://www.mintscan.io/kava</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>aave</t>
+          <t>elrond-egld</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -2478,45 +2482,45 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>14393945.57755076</v>
+        <v>24184559.18984154</v>
       </c>
       <c r="F46" t="n">
-        <v>16000000</v>
+        <v>31415926</v>
       </c>
       <c r="G46" t="n">
-        <v>935794982.448364</v>
+        <v>878503233.9950291</v>
       </c>
       <c r="H46" t="n">
-        <v>17444837.88282198</v>
+        <v>5316411.719507685</v>
       </c>
       <c r="I46" t="n">
-        <v>65.013097166899</v>
+        <v>36.324963672029</v>
       </c>
       <c r="J46" t="n">
-        <v>-1.7028669375091</v>
+        <v>-2.137663523946544</v>
       </c>
       <c r="K46" t="n">
-        <v>65.41799919414233</v>
+        <v>36.52162538028627</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x80fB784B7eD66730e8b1DBd9820aFD29931aab03</t>
+          <t>https://explorer.elrond.com/</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>theta</t>
+          <t>render-token</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -2524,38 +2528,38 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>THETA</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>THETA</t>
+          <t>Render Token</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>1000000000</v>
+        <v>366378124.108796</v>
       </c>
       <c r="F47" t="n">
-        <v>1000000000</v>
+        <v>536870912</v>
       </c>
       <c r="G47" t="n">
-        <v>915177623.8887436</v>
+        <v>875851628.7784848</v>
       </c>
       <c r="H47" t="n">
-        <v>3386713.256040845</v>
+        <v>36642441.13334316</v>
       </c>
       <c r="I47" t="n">
-        <v>0.9151776238887436</v>
+        <v>2.390567479728677</v>
       </c>
       <c r="J47" t="n">
-        <v>-1.617309020897653</v>
+        <v>1.01877452435781</v>
       </c>
       <c r="K47" t="n">
-        <v>0.914781957841076</v>
+        <v>2.508335061542458</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>https://explorer.thetatoken.org/</t>
+          <t>https://etherscan.io/token/0x6de037ef9ad2725eb40118bb1702ebb27e4aeb24</t>
         </is>
       </c>
     </row>
@@ -2579,25 +2583,25 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>1380744515.7246</v>
+        <v>1381123664.695468</v>
       </c>
       <c r="F48" t="n">
         <v>1818000000</v>
       </c>
       <c r="G48" t="n">
-        <v>907310344.2188296</v>
+        <v>875062188.7038075</v>
       </c>
       <c r="H48" t="n">
-        <v>9827299.425154941</v>
+        <v>6300371.57905988</v>
       </c>
       <c r="I48" t="n">
-        <v>0.6571167467159433</v>
+        <v>0.6335871371060426</v>
       </c>
       <c r="J48" t="n">
-        <v>-1.374343117704924</v>
+        <v>-4.624402106521336</v>
       </c>
       <c r="K48" t="n">
-        <v>0.6571260211203069</v>
+        <v>0.6439217082542364</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
@@ -2608,7 +2612,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>elrond-egld</t>
+          <t>theta</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -2616,45 +2620,45 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>THETA</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>THETA</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>24184559.18984154</v>
+        <v>1000000000</v>
       </c>
       <c r="F49" t="n">
-        <v>31415926</v>
+        <v>1000000000</v>
       </c>
       <c r="G49" t="n">
-        <v>894063411.4081435</v>
+        <v>857075850.9391611</v>
       </c>
       <c r="H49" t="n">
-        <v>5261293.399243087</v>
+        <v>6279072.179876389</v>
       </c>
       <c r="I49" t="n">
-        <v>36.96835672670375</v>
+        <v>0.8570758509391611</v>
       </c>
       <c r="J49" t="n">
-        <v>-1.89452178443522</v>
+        <v>-3.080730702317335</v>
       </c>
       <c r="K49" t="n">
-        <v>37.11745265264497</v>
+        <v>0.857885230921809</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>https://explorer.elrond.com/</t>
+          <t>https://explorer.thetatoken.org/</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>conflux-network</t>
+          <t>frax</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -2662,43 +2666,43 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CFX</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Conflux</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>2879955431.201849</v>
+        <v>1004141409.408784</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="n">
-        <v>893722701.6262423</v>
+        <v>854058702.7919453</v>
       </c>
       <c r="H50" t="n">
-        <v>65677200.56579298</v>
+        <v>2090248.111687792</v>
       </c>
       <c r="I50" t="n">
-        <v>0.31032518487735</v>
+        <v>0.8505362838236058</v>
       </c>
       <c r="J50" t="n">
-        <v>1.559007190430974</v>
+        <v>-14.92662673727729</v>
       </c>
       <c r="K50" t="n">
-        <v>0.3000726686250472</v>
+        <v>0.9898534526893537</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>http://www.confluxscan.io/</t>
+          <t>https://etherscan.io/token/0x853d955acef822db058eb8505911ed77f175b99e</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>render-token</t>
+          <t>tezos</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -2706,45 +2710,43 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>XTZ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Render Token</t>
+          <t>Tezos</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>363911539.108796</v>
-      </c>
-      <c r="F51" t="n">
-        <v>536870912</v>
-      </c>
+        <v>938751773.8098899</v>
+      </c>
+      <c r="F51" t="inlineStr"/>
       <c r="G51" t="n">
-        <v>886186218.6297637</v>
+        <v>839597938.1074063</v>
       </c>
       <c r="H51" t="n">
-        <v>34829525.56334516</v>
+        <v>7105667.193305033</v>
       </c>
       <c r="I51" t="n">
-        <v>2.435169329337554</v>
+        <v>0.8943769391773594</v>
       </c>
       <c r="J51" t="n">
-        <v>4.142647295678495</v>
+        <v>-0.8969594926076641</v>
       </c>
       <c r="K51" t="n">
-        <v>2.374620724003425</v>
+        <v>0.8974445471075885</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x6de037ef9ad2725eb40118bb1702ebb27e4aeb24</t>
+          <t>https://tzkt.io/</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>kava</t>
+          <t>conflux-network</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -2752,43 +2754,43 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>KAVA</t>
+          <t>CFX</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Kava</t>
+          <t>Conflux</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>525037471</v>
+        <v>2880719900.091294</v>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="n">
-        <v>868427565.3978947</v>
+        <v>837058694.6170272</v>
       </c>
       <c r="H52" t="n">
-        <v>18169519.36319898</v>
+        <v>50595770.01147359</v>
       </c>
       <c r="I52" t="n">
-        <v>1.65402969000263</v>
+        <v>0.290572746968735</v>
       </c>
       <c r="J52" t="n">
-        <v>-4.060327516877019</v>
+        <v>-1.939073550172937</v>
       </c>
       <c r="K52" t="n">
-        <v>1.292819596971424</v>
+        <v>0.2983612020063007</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>https://www.mintscan.io/kava</t>
+          <t>http://www.confluxscan.io/</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>tezos</t>
+          <t>axie-infinity</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -2796,43 +2798,45 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>XTZ</t>
+          <t>AXS</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Tezos</t>
+          <t>Axie Infinity</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>938403110.2527449</v>
-      </c>
-      <c r="F53" t="inlineStr"/>
+        <v>116956335.3265201</v>
+      </c>
+      <c r="F53" t="n">
+        <v>270000000</v>
+      </c>
       <c r="G53" t="n">
-        <v>834488680.1399565</v>
+        <v>800933764.1536592</v>
       </c>
       <c r="H53" t="n">
-        <v>7627951.795978779</v>
+        <v>8594982.51231296</v>
       </c>
       <c r="I53" t="n">
-        <v>0.8892646145590878</v>
+        <v>6.848143470959505</v>
       </c>
       <c r="J53" t="n">
-        <v>-2.357628783490931</v>
+        <v>-2.670180169026273</v>
       </c>
       <c r="K53" t="n">
-        <v>0.8978382414528372</v>
+        <v>6.867635162987037</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>https://tzkt.io/</t>
+          <t>https://etherscan.io/token/0xf5d669627376ebd411e34b98f19c868c8aba5ada</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>axie-infinity</t>
+          <t>flow</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -2840,45 +2844,43 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>AXS</t>
+          <t>FLOW</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Axie Infinity</t>
+          <t>Flow</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>116956335.3265201</v>
-      </c>
-      <c r="F54" t="n">
-        <v>270000000</v>
-      </c>
+        <v>1036200000</v>
+      </c>
+      <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
-        <v>818162234.6509053</v>
+        <v>776063382.1817751</v>
       </c>
       <c r="H54" t="n">
-        <v>20800382.0917522</v>
+        <v>1882946.269109189</v>
       </c>
       <c r="I54" t="n">
-        <v>6.995450330815769</v>
+        <v>0.7489513435454306</v>
       </c>
       <c r="J54" t="n">
-        <v>-3.333198990359348</v>
+        <v>-2.52054302230202</v>
       </c>
       <c r="K54" t="n">
-        <v>7.106104394594122</v>
+        <v>0.7506096094373439</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xf5d669627376ebd411e34b98f19c868c8aba5ada</t>
+          <t>https://flowscan.org/</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>flow</t>
+          <t>hedera-hashgraph</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -2886,43 +2888,45 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>FLOW</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Flow</t>
+          <t>Hedera Hashgraph</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>1036200000</v>
-      </c>
-      <c r="F55" t="inlineStr"/>
+        <v>14832756028</v>
+      </c>
+      <c r="F55" t="n">
+        <v>50000000000</v>
+      </c>
       <c r="G55" t="n">
-        <v>799427741.1610864</v>
+        <v>774782686.2628975</v>
       </c>
       <c r="H55" t="n">
-        <v>3224090.317630921</v>
+        <v>3759354.164481339</v>
       </c>
       <c r="I55" t="n">
-        <v>0.7714994606843143</v>
+        <v>0.0522345735883695</v>
       </c>
       <c r="J55" t="n">
-        <v>-2.155800600011757</v>
+        <v>-1.34344200027415</v>
       </c>
       <c r="K55" t="n">
-        <v>0.7754512118598967</v>
+        <v>0.0524319855733724</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>https://flowscan.org/</t>
+          <t>https://hash-hash.info/</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>hedera-hashgraph</t>
+          <t>chiliz</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -2930,45 +2934,45 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>CHZ</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Hedera Hashgraph</t>
+          <t>Chiliz</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>14832756028</v>
+        <v>6975647158.46161</v>
       </c>
       <c r="F56" t="n">
-        <v>50000000000</v>
+        <v>8888888888</v>
       </c>
       <c r="G56" t="n">
-        <v>778408067.8890195</v>
+        <v>725255428.7357768</v>
       </c>
       <c r="H56" t="n">
-        <v>4953256.584001674</v>
+        <v>9540736.265451889</v>
       </c>
       <c r="I56" t="n">
-        <v>0.0524789908510332</v>
+        <v>0.1039696263673581</v>
       </c>
       <c r="J56" t="n">
-        <v>-0.4614766679773859</v>
+        <v>-2.882363417505551</v>
       </c>
       <c r="K56" t="n">
-        <v>0.052301180733562</v>
+        <v>0.1046820247940436</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>https://hash-hash.info/</t>
+          <t>https://etherscan.io/token/0x3506424f91fd33084466f402d5d97f05f8e3b4af</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>chiliz</t>
+          <t>kucoin-token</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -2976,45 +2980,45 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CHZ</t>
+          <t>KCS</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Chiliz</t>
+          <t>KuCoin Token</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>6975647158.46161</v>
+        <v>96974735.45697574</v>
       </c>
       <c r="F57" t="n">
-        <v>8888888888</v>
+        <v>170118638</v>
       </c>
       <c r="G57" t="n">
-        <v>750452129.4447091</v>
+        <v>713520173.271902</v>
       </c>
       <c r="H57" t="n">
-        <v>11256526.30066698</v>
+        <v>837456.2636552484</v>
       </c>
       <c r="I57" t="n">
-        <v>0.1075817214370418</v>
+        <v>7.357794480279512</v>
       </c>
       <c r="J57" t="n">
-        <v>-0.4790357697681298</v>
+        <v>-0.9885992269399124</v>
       </c>
       <c r="K57" t="n">
-        <v>0.1070561825642046</v>
+        <v>7.380991567430714</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x3506424f91fd33084466f402d5d97f05f8e3b4af</t>
+          <t>https://etherscan.io/token/0xf34960d9d60be18cc1d5afc1a6f012a723a28811</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>kucoin-token</t>
+          <t>curve-dao-token</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -3022,38 +3026,38 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>KCS</t>
+          <t>CRV</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>KuCoin Token</t>
+          <t>Curve DAO Token</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>96974735.45697574</v>
+        <v>818212083</v>
       </c>
       <c r="F58" t="n">
-        <v>170118638</v>
+        <v>3303030299</v>
       </c>
       <c r="G58" t="n">
-        <v>723021757.5737058</v>
+        <v>688685702.0382676</v>
       </c>
       <c r="H58" t="n">
-        <v>1030103.360868901</v>
+        <v>5801122.095591295</v>
       </c>
       <c r="I58" t="n">
-        <v>7.455774477409995</v>
+        <v>0.8416958345483974</v>
       </c>
       <c r="J58" t="n">
-        <v>-0.1869687348926519</v>
+        <v>1.667931888441588</v>
       </c>
       <c r="K58" t="n">
-        <v>7.456100775181103</v>
+        <v>0.8338727896105297</v>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xf34960d9d60be18cc1d5afc1a6f012a723a28811</t>
+          <t>https://etherscan.io/token/0xD533a949740bb3306d119CC777fa900bA034cd52</t>
         </is>
       </c>
     </row>
@@ -3083,19 +3087,19 @@
         <v>21000000</v>
       </c>
       <c r="G59" t="n">
-        <v>682745470.9167933</v>
+        <v>679705679.766506</v>
       </c>
       <c r="H59" t="n">
-        <v>28748817.21219132</v>
+        <v>31897337.52918632</v>
       </c>
       <c r="I59" t="n">
-        <v>41.8137085670392</v>
+        <v>41.62754117863879</v>
       </c>
       <c r="J59" t="n">
-        <v>-4.276461083279317</v>
+        <v>-0.894409457304202</v>
       </c>
       <c r="K59" t="n">
-        <v>42.03467741775371</v>
+        <v>39.62838646692106</v>
       </c>
       <c r="L59" t="inlineStr">
         <is>
@@ -3106,7 +3110,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>curve-dao-token</t>
+          <t>bitcoin-sv</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -3114,38 +3118,38 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CRV</t>
+          <t>BSV</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Curve DAO Token</t>
+          <t>Bitcoin SV</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>817700222</v>
+        <v>19266076.64423905</v>
       </c>
       <c r="F60" t="n">
-        <v>3303030299</v>
+        <v>21000000</v>
       </c>
       <c r="G60" t="n">
-        <v>677881868.2983245</v>
+        <v>671989677.1447688</v>
       </c>
       <c r="H60" t="n">
-        <v>5916673.07318417</v>
+        <v>10493690.8168004</v>
       </c>
       <c r="I60" t="n">
-        <v>0.8290102534646548</v>
+        <v>34.87942509279426</v>
       </c>
       <c r="J60" t="n">
-        <v>0.2826755887580594</v>
+        <v>-0.7440530659069637</v>
       </c>
       <c r="K60" t="n">
-        <v>0.8207578508741799</v>
+        <v>34.56262470903608</v>
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xD533a949740bb3306d119CC777fa900bA034cd52</t>
+          <t>https://bsvexplorer.io/</t>
         </is>
       </c>
     </row>
@@ -3175,19 +3179,19 @@
         <v>100000000</v>
       </c>
       <c r="G61" t="n">
-        <v>669782441.5028464</v>
+        <v>660001751.51863</v>
       </c>
       <c r="H61" t="n">
-        <v>9349516.679600701</v>
+        <v>13401442.67768633</v>
       </c>
       <c r="I61" t="n">
-        <v>9.495230244216073</v>
+        <v>9.356573424340278</v>
       </c>
       <c r="J61" t="n">
-        <v>-1.069505360911056</v>
+        <v>-1.352632528053412</v>
       </c>
       <c r="K61" t="n">
-        <v>9.516443743953937</v>
+        <v>9.274542582950399</v>
       </c>
       <c r="L61" t="inlineStr">
         <is>
@@ -3198,7 +3202,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>bitcoin-sv</t>
+          <t>maker</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -3206,45 +3210,45 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>BSV</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Bitcoin SV</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>19266076.64423905</v>
+        <v>977631.03695089</v>
       </c>
       <c r="F62" t="n">
-        <v>21000000</v>
+        <v>1005577</v>
       </c>
       <c r="G62" t="n">
-        <v>651380346.7095277</v>
+        <v>610018030.2909323</v>
       </c>
       <c r="H62" t="n">
-        <v>11145349.2805979</v>
+        <v>3622508.499809942</v>
       </c>
       <c r="I62" t="n">
-        <v>33.80970390275613</v>
+        <v>623.9757201177889</v>
       </c>
       <c r="J62" t="n">
-        <v>-0.9555215185421904</v>
+        <v>-0.3002743248142722</v>
       </c>
       <c r="K62" t="n">
-        <v>33.693044973227</v>
+        <v>622.7734150799529</v>
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>https://bsvexplorer.io/</t>
+          <t>https://etherscan.io/token/Maker</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>maker</t>
+          <t>synthetix-network-token</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -3252,45 +3256,45 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>SNX</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Synthetix</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>977631.03695089</v>
+        <v>233716733.49</v>
       </c>
       <c r="F63" t="n">
-        <v>1005577</v>
+        <v>212424133</v>
       </c>
       <c r="G63" t="n">
-        <v>613445615.3054222</v>
+        <v>554571808.7444649</v>
       </c>
       <c r="H63" t="n">
-        <v>4387029.510472225</v>
+        <v>7396147.289937006</v>
       </c>
       <c r="I63" t="n">
-        <v>627.481730959241</v>
+        <v>2.37283741075473</v>
       </c>
       <c r="J63" t="n">
-        <v>-1.908071252169115</v>
+        <v>-0.06628687825177659</v>
       </c>
       <c r="K63" t="n">
-        <v>630.2042780241183</v>
+        <v>2.358690005022457</v>
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/Maker</t>
+          <t>https://etherscan.io/token/0xc011a72400e58ecd99ee497cf89e3775d4bd732f</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>synthetix-network-token</t>
+          <t>klaytn</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -3298,45 +3302,43 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SNX</t>
+          <t>KLAY</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Synthetix</t>
+          <t>Klaytn</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>233716733.49</v>
-      </c>
-      <c r="F64" t="n">
-        <v>212424133</v>
-      </c>
+        <v>3094961001.842067</v>
+      </c>
+      <c r="F64" t="inlineStr"/>
       <c r="G64" t="n">
-        <v>556927755.7421279</v>
+        <v>545022622.7405559</v>
       </c>
       <c r="H64" t="n">
-        <v>16140687.44297908</v>
+        <v>3821622.162993413</v>
       </c>
       <c r="I64" t="n">
-        <v>2.382917762993453</v>
+        <v>0.1760999968710972</v>
       </c>
       <c r="J64" t="n">
-        <v>-1.703792946074918</v>
+        <v>-2.644100067651649</v>
       </c>
       <c r="K64" t="n">
-        <v>2.399475007774492</v>
+        <v>0.1768968241530179</v>
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xc011a72400e58ecd99ee497cf89e3775d4bd732f</t>
+          <t>https://scope.klaytn.com/blocks</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>klaytn</t>
+          <t>casper</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -3344,43 +3346,43 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>KLAY</t>
+          <t>CSPR</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Klaytn</t>
+          <t>Casper</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>3094194574.010779</v>
+        <v>11027543425</v>
       </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="n">
-        <v>548631518.7964165</v>
+        <v>533740050.803842</v>
       </c>
       <c r="H65" t="n">
-        <v>5853495.840972562</v>
+        <v>1403560.88750238</v>
       </c>
       <c r="I65" t="n">
-        <v>0.1773099608552624</v>
+        <v>0.0484006301524804</v>
       </c>
       <c r="J65" t="n">
-        <v>-2.6993448825318</v>
+        <v>-2.960935926731245</v>
       </c>
       <c r="K65" t="n">
-        <v>0.1777624255954499</v>
+        <v>0.0494934873534371</v>
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>https://scope.klaytn.com/blocks</t>
+          <t>https://casperstats.io/</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>casper</t>
+          <t>frax-share</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -3388,36 +3390,36 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CSPR</t>
+          <t>FXS</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Casper</t>
+          <t>Frax Share</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>11021271985</v>
+        <v>72141875.39783853</v>
       </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="n">
-        <v>521281363.7355573</v>
+        <v>511882233.4232361</v>
       </c>
       <c r="H66" t="n">
-        <v>1728629.353468438</v>
+        <v>636252.9447139807</v>
       </c>
       <c r="I66" t="n">
-        <v>0.0472977497012163</v>
+        <v>7.095493852916565</v>
       </c>
       <c r="J66" t="n">
-        <v>-1.33965826185036</v>
+        <v>-1.721192790062559</v>
       </c>
       <c r="K66" t="n">
-        <v>0.0474035927413435</v>
+        <v>7.128099302846059</v>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>https://casperstats.io/</t>
+          <t>https://etherscan.io/token/0x3432b6a60d23ca0dfca7761b7ab56459d9c964d0</t>
         </is>
       </c>
     </row>
@@ -3441,23 +3443,23 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>902802371.8400393</v>
+        <v>904398960.8400393</v>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="n">
-        <v>518974298.6665016</v>
+        <v>507027398.316371</v>
       </c>
       <c r="H67" t="n">
-        <v>5714136.401538641</v>
+        <v>5632341.140634382</v>
       </c>
       <c r="I67" t="n">
-        <v>0.574848178133115</v>
+        <v>0.5606235967425539</v>
       </c>
       <c r="J67" t="n">
-        <v>-2.461934149131726</v>
+        <v>-3.626439831661403</v>
       </c>
       <c r="K67" t="n">
-        <v>0.5779543789766793</v>
+        <v>0.5694874604780037</v>
       </c>
       <c r="L67" t="inlineStr">
         <is>
@@ -3468,7 +3470,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>frax-share</t>
+          <t>injective-protocol</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -3476,36 +3478,38 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>FXS</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Frax Share</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>71926470.00299317</v>
-      </c>
-      <c r="F68" t="inlineStr"/>
+        <v>73005554.33</v>
+      </c>
+      <c r="F68" t="n">
+        <v>100000000</v>
+      </c>
       <c r="G68" t="n">
-        <v>518089668.9773059</v>
+        <v>504618558.4344536</v>
       </c>
       <c r="H68" t="n">
-        <v>774549.5254621673</v>
+        <v>25208067.21504452</v>
       </c>
       <c r="I68" t="n">
-        <v>7.203045957291466</v>
+        <v>6.912057076554404</v>
       </c>
       <c r="J68" t="n">
-        <v>-1.489477568371464</v>
+        <v>-1.867328767119261</v>
       </c>
       <c r="K68" t="n">
-        <v>7.225690701395592</v>
+        <v>6.882101554135917</v>
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x3432b6a60d23ca0dfca7761b7ab56459d9c964d0</t>
+          <t>https://etherscan.io/token/0xe28b3b32b6c345a34ff64674606124dd5aceca30</t>
         </is>
       </c>
     </row>
@@ -3529,25 +3533,25 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>19391410923303</v>
+        <v>19394017173303</v>
       </c>
       <c r="F69" t="n">
         <v>21000000000000</v>
       </c>
       <c r="G69" t="n">
-        <v>506797558.7166436</v>
+        <v>502157119.750206</v>
       </c>
       <c r="H69" t="n">
-        <v>1490698.976127425</v>
+        <v>1135702.745399804</v>
       </c>
       <c r="I69" t="n">
-        <v>2.61351564732e-05</v>
+        <v>2.58923726458e-05</v>
       </c>
       <c r="J69" t="n">
-        <v>-0.6950825341827978</v>
+        <v>-0.8921727943533708</v>
       </c>
       <c r="K69" t="n">
-        <v>2.60287328199e-05</v>
+        <v>2.57157112655e-05</v>
       </c>
       <c r="L69" t="inlineStr">
         <is>
@@ -3581,19 +3585,19 @@
         <v>2779530283</v>
       </c>
       <c r="G70" t="n">
-        <v>504703711.6681757</v>
+        <v>500252649.2076753</v>
       </c>
       <c r="H70" t="n">
-        <v>4285093.611288421</v>
+        <v>2809145.310554536</v>
       </c>
       <c r="I70" t="n">
-        <v>0.1815787778082559</v>
+        <v>0.1799774056311929</v>
       </c>
       <c r="J70" t="n">
-        <v>-2.00586828661887</v>
+        <v>1.509411011077592</v>
       </c>
       <c r="K70" t="n">
-        <v>0.1829019082695045</v>
+        <v>0.1762066121549329</v>
       </c>
       <c r="L70" t="inlineStr">
         <is>
@@ -3604,7 +3608,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>injective-protocol</t>
+          <t>dash</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -3612,45 +3616,45 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>DASH</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Dash</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>73005554.33</v>
+        <v>11286362.82185394</v>
       </c>
       <c r="F71" t="n">
-        <v>100000000</v>
+        <v>18900000</v>
       </c>
       <c r="G71" t="n">
-        <v>499674941.9809989</v>
+        <v>498504916.4124929</v>
       </c>
       <c r="H71" t="n">
-        <v>31190428.96683675</v>
+        <v>29649686.46240984</v>
       </c>
       <c r="I71" t="n">
-        <v>6.84434145547839</v>
+        <v>44.16878353823881</v>
       </c>
       <c r="J71" t="n">
-        <v>3.978976976220515</v>
+        <v>-1.71887675414678</v>
       </c>
       <c r="K71" t="n">
-        <v>6.576590464175321</v>
+        <v>43.65476430468968</v>
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xe28b3b32b6c345a34ff64674606124dd5aceca30</t>
+          <t>https://explorer.dash.org</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>dash</t>
+          <t>gatetoken</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -3658,45 +3662,39 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>DASH</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Dash</t>
+          <t>GateToken</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>11282507.44575294</v>
-      </c>
-      <c r="F72" t="n">
-        <v>18900000</v>
-      </c>
+        <v>97787093.7551627</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
       <c r="G72" t="n">
-        <v>499640360.1245555</v>
+        <v>480567258.6954134</v>
       </c>
       <c r="H72" t="n">
-        <v>37976513.80673383</v>
+        <v>303653.676661814</v>
       </c>
       <c r="I72" t="n">
-        <v>44.2845141052962</v>
+        <v>4.914424186678947</v>
       </c>
       <c r="J72" t="n">
-        <v>-0.5657270923095143</v>
+        <v>-0.4598846667950171</v>
       </c>
       <c r="K72" t="n">
-        <v>43.60292215800255</v>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>https://explorer.dash.org</t>
-        </is>
-      </c>
+        <v>4.904090851134876</v>
+      </c>
+      <c r="L72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>gatetoken</t>
+          <t>huobi-token</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -3704,39 +3702,45 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>HT</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>GateToken</t>
+          <t>Huobi Token</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>97786860.58951971</v>
-      </c>
-      <c r="F73" t="inlineStr"/>
+        <v>162233844</v>
+      </c>
+      <c r="F73" t="n">
+        <v>500000000</v>
+      </c>
       <c r="G73" t="n">
-        <v>475947770.254575</v>
+        <v>476310980.2870722</v>
       </c>
       <c r="H73" t="n">
-        <v>473576.8913451841</v>
+        <v>15592855.64232934</v>
       </c>
       <c r="I73" t="n">
-        <v>4.867195524892273</v>
+        <v>2.935953242204334</v>
       </c>
       <c r="J73" t="n">
-        <v>-0.6716969683105166</v>
+        <v>1.009644000187059</v>
       </c>
       <c r="K73" t="n">
-        <v>4.861456528343697</v>
-      </c>
-      <c r="L73" t="inlineStr"/>
+        <v>2.923731286980715</v>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>https://etherscan.io/token/0x6f259637dcd74c767781e37bc6133cd6a68aa161</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>huobi-token</t>
+          <t>trust-wallet-token</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -3744,45 +3748,45 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>HT</t>
+          <t>TWT</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Huobi Token</t>
+          <t>Trust Wallet Token</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>162233844</v>
+        <v>416649900</v>
       </c>
       <c r="F74" t="n">
-        <v>500000000</v>
+        <v>1000000000</v>
       </c>
       <c r="G74" t="n">
-        <v>473349497.3043288</v>
+        <v>446640259.8448671</v>
       </c>
       <c r="H74" t="n">
-        <v>17053779.04744208</v>
+        <v>1677193.804089612</v>
       </c>
       <c r="I74" t="n">
-        <v>2.917698832953307</v>
+        <v>1.071979760093227</v>
       </c>
       <c r="J74" t="n">
-        <v>-0.8298145113045607</v>
+        <v>-1.597146894283919</v>
       </c>
       <c r="K74" t="n">
-        <v>2.908016492580675</v>
+        <v>1.069274482886701</v>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x6f259637dcd74c767781e37bc6133cd6a68aa161</t>
+          <t>https://explorer.binance.org/asset/TWT-8C2</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>trust-wallet-token</t>
+          <t>fei-protocol</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -3790,38 +3794,36 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>TWT</t>
+          <t>FEI</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Trust Wallet Token</t>
+          <t>Fei Protocol</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>416649900</v>
-      </c>
-      <c r="F75" t="n">
-        <v>1000000000</v>
-      </c>
+        <v>424996177.7889056</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
       <c r="G75" t="n">
-        <v>458442546.2137943</v>
+        <v>411389914.0273101</v>
       </c>
       <c r="H75" t="n">
-        <v>2894238.767847089</v>
+        <v>451178.2274324044</v>
       </c>
       <c r="I75" t="n">
-        <v>1.100306387242129</v>
+        <v>0.9679849738122736</v>
       </c>
       <c r="J75" t="n">
-        <v>-0.5455534272911339</v>
+        <v>7.520220347258458</v>
       </c>
       <c r="K75" t="n">
-        <v>1.11007122451655</v>
+        <v>0.96287786090461</v>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>https://explorer.binance.org/asset/TWT-8C2</t>
+          <t>https://etherscan.io/token/0x956F47F50A910163D8BF957Cf5846D573E7f87CA</t>
         </is>
       </c>
     </row>
@@ -3849,19 +3851,19 @@
       </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="n">
-        <v>397734115.2401397</v>
+        <v>398990832.0373255</v>
       </c>
       <c r="H76" t="n">
-        <v>1124199.133337915</v>
+        <v>1075594.199841798</v>
       </c>
       <c r="I76" t="n">
-        <v>0.0323537475648798</v>
+        <v>0.0324559754011622</v>
       </c>
       <c r="J76" t="n">
-        <v>-0.4201225491328003</v>
+        <v>1.954319295466455</v>
       </c>
       <c r="K76" t="n">
-        <v>0.0316929985528222</v>
+        <v>0.0322299330089857</v>
       </c>
       <c r="L76" t="inlineStr">
         <is>
@@ -3895,19 +3897,19 @@
         <v>1374513896</v>
       </c>
       <c r="G77" t="n">
-        <v>396819562.5053806</v>
+        <v>388019409.9006872</v>
       </c>
       <c r="H77" t="n">
-        <v>3412288.618747339</v>
+        <v>2553276.894165872</v>
       </c>
       <c r="I77" t="n">
-        <v>0.2980399149124585</v>
+        <v>0.2914303699672445</v>
       </c>
       <c r="J77" t="n">
-        <v>-1.249410421254618</v>
+        <v>-2.078368966975818</v>
       </c>
       <c r="K77" t="n">
-        <v>0.2981441344227852</v>
+        <v>0.2923422414110217</v>
       </c>
       <c r="L77" t="inlineStr">
         <is>
@@ -3918,7 +3920,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>wootrade</t>
+          <t>pancakeswap</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -3926,43 +3928,45 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>WOO</t>
+          <t>CAKE</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>WOO Network</t>
+          <t>PancakeSwap</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>1694236239.524501</v>
-      </c>
-      <c r="F78" t="inlineStr"/>
+        <v>209557428.6183616</v>
+      </c>
+      <c r="F78" t="n">
+        <v>750000000</v>
+      </c>
       <c r="G78" t="n">
-        <v>391133721.0075225</v>
+        <v>378312937.0842447</v>
       </c>
       <c r="H78" t="n">
-        <v>2114644.569682429</v>
+        <v>4149953.65401274</v>
       </c>
       <c r="I78" t="n">
-        <v>0.2308613827769951</v>
+        <v>1.805294804285915</v>
       </c>
       <c r="J78" t="n">
-        <v>-2.477893227284469</v>
+        <v>-1.976648086277129</v>
       </c>
       <c r="K78" t="n">
-        <v>0.2308606327847112</v>
+        <v>1.814356086272392</v>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x4691937a7508860f876c9c0a2a617e7d9e945d4b</t>
+          <t>https://bscscan.com/token/0x0e09fabb73bd3ade0a17ecc321fd13a19e81ce82</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>fei-protocol</t>
+          <t>wootrade</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -3970,36 +3974,36 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>FEI</t>
+          <t>WOO</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Fei Protocol</t>
+          <t>WOO Network</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>424996177.7889056</v>
+        <v>1694310805.018443</v>
       </c>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="n">
-        <v>384124979.2775705</v>
+        <v>372312475.5786151</v>
       </c>
       <c r="H79" t="n">
-        <v>1072668.091137041</v>
+        <v>1700505.273486027</v>
       </c>
       <c r="I79" t="n">
-        <v>0.9038316092065288</v>
+        <v>0.2197427263497634</v>
       </c>
       <c r="J79" t="n">
-        <v>0.1015002470301621</v>
+        <v>-3.037064201244869</v>
       </c>
       <c r="K79" t="n">
-        <v>0.9441366218942188</v>
+        <v>0.2239814456948951</v>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x956F47F50A910163D8BF957Cf5846D573E7f87CA</t>
+          <t>https://etherscan.io/token/0x4691937a7508860f876c9c0a2a617e7d9e945d4b</t>
         </is>
       </c>
     </row>
@@ -4029,19 +4033,19 @@
         <v>21000000000</v>
       </c>
       <c r="G80" t="n">
-        <v>383428849.6419407</v>
+        <v>368183904.5528416</v>
       </c>
       <c r="H80" t="n">
-        <v>9107775.992093442</v>
+        <v>7228919.875519221</v>
       </c>
       <c r="I80" t="n">
-        <v>0.0241641109303966</v>
+        <v>0.0232033576000074</v>
       </c>
       <c r="J80" t="n">
-        <v>-1.836816103947248</v>
+        <v>-3.687454203610168</v>
       </c>
       <c r="K80" t="n">
-        <v>0.0241473643287273</v>
+        <v>0.0235059673182561</v>
       </c>
       <c r="L80" t="inlineStr">
         <is>
@@ -4069,25 +4073,25 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>327448958</v>
+        <v>329138015</v>
       </c>
       <c r="F81" t="n">
         <v>500000000</v>
       </c>
       <c r="G81" t="n">
-        <v>382546070.5963612</v>
+        <v>365274251.739138</v>
       </c>
       <c r="H81" t="n">
-        <v>6092306.860787408</v>
+        <v>4651808.813934336</v>
       </c>
       <c r="I81" t="n">
-        <v>1.168261682470711</v>
+        <v>1.109790528873239</v>
       </c>
       <c r="J81" t="n">
-        <v>-2.309159687251298</v>
+        <v>-2.932587119857739</v>
       </c>
       <c r="K81" t="n">
-        <v>1.178008463333823</v>
+        <v>1.121404102859951</v>
       </c>
       <c r="L81" t="inlineStr">
         <is>
@@ -4098,7 +4102,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>pancakeswap</t>
+          <t>nexo</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -4106,38 +4110,38 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>CAKE</t>
+          <t>NEXO</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>PancakeSwap</t>
+          <t>Nexo</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>201063168.7488464</v>
+        <v>560000011</v>
       </c>
       <c r="F82" t="n">
-        <v>750000000</v>
+        <v>1000000000</v>
       </c>
       <c r="G82" t="n">
-        <v>369497118.089739</v>
+        <v>361063069.900718</v>
       </c>
       <c r="H82" t="n">
-        <v>5796806.09379489</v>
+        <v>318066.4062717216</v>
       </c>
       <c r="I82" t="n">
-        <v>1.83771657628299</v>
+        <v>0.6447554693007282</v>
       </c>
       <c r="J82" t="n">
-        <v>-1.810542640484572</v>
+        <v>-1.113938121217757</v>
       </c>
       <c r="K82" t="n">
-        <v>1.843446501293994</v>
+        <v>0.6730948632789892</v>
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>https://bscscan.com/token/0x0e09fabb73bd3ade0a17ecc321fd13a19e81ce82</t>
+          <t>https://etherscan.io/token/0xb62132e35a6c13ee1ee0f84dc5d40bad8d815206</t>
         </is>
       </c>
     </row>
@@ -4167,19 +4171,19 @@
         <v>100000000</v>
       </c>
       <c r="G83" t="n">
-        <v>367401708.1596436</v>
+        <v>347834988.0295669</v>
       </c>
       <c r="H83" t="n">
-        <v>71152158.3939192</v>
+        <v>29096163.26133512</v>
       </c>
       <c r="I83" t="n">
-        <v>4.585356732101636</v>
+        <v>4.341154296780865</v>
       </c>
       <c r="J83" t="n">
-        <v>3.466607521589813</v>
+        <v>-5.360219460151922</v>
       </c>
       <c r="K83" t="n">
-        <v>4.604408523959833</v>
+        <v>4.523952151472594</v>
       </c>
       <c r="L83" t="inlineStr">
         <is>
@@ -4207,25 +4211,25 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>77317829.37396598</v>
+        <v>77346251.36926366</v>
       </c>
       <c r="F84" t="n">
         <v>100000000</v>
       </c>
       <c r="G84" t="n">
-        <v>365031145.2395843</v>
+        <v>344924028.1981229</v>
       </c>
       <c r="H84" t="n">
-        <v>1672427.25053766</v>
+        <v>212523.5619563461</v>
       </c>
       <c r="I84" t="n">
-        <v>4.721176838449832</v>
+        <v>4.459479575181985</v>
       </c>
       <c r="J84" t="n">
-        <v>-3.020765240916889</v>
+        <v>-3.236568375547492</v>
       </c>
       <c r="K84" t="n">
-        <v>4.677253608124307</v>
+        <v>4.510136280856896</v>
       </c>
       <c r="L84" t="inlineStr">
         <is>
@@ -4236,7 +4240,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>ftx-token</t>
+          <t>enjin-coin</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -4244,45 +4248,45 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>FTT</t>
+          <t>ENJ</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>FTX Token</t>
+          <t>Enjin Coin</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>328895103.813207</v>
+        <v>1000000000</v>
       </c>
       <c r="F85" t="n">
-        <v>352170015</v>
+        <v>1000000000</v>
       </c>
       <c r="G85" t="n">
-        <v>360025963.3843138</v>
+        <v>338953645.2120961</v>
       </c>
       <c r="H85" t="n">
-        <v>2226305.706048379</v>
+        <v>2523499.275122396</v>
       </c>
       <c r="I85" t="n">
-        <v>1.0946528519585</v>
+        <v>0.3389536452120961</v>
       </c>
       <c r="J85" t="n">
-        <v>-3.687400134827228</v>
+        <v>-1.478234986396599</v>
       </c>
       <c r="K85" t="n">
-        <v>1.106063896759088</v>
+        <v>0.3399964841499848</v>
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x50d1c9771902476076ecfc8b2a83ad6b9355a4c9</t>
+          <t>https://etherscan.io/token/0xf629cbd94d3791c9250152bd8dfbdf380e2a3b9c</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>nexo</t>
+          <t>ftx-token</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -4290,45 +4294,45 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>NEXO</t>
+          <t>FTT</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Nexo</t>
+          <t>FTX Token</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>560000011</v>
+        <v>328895103.813207</v>
       </c>
       <c r="F86" t="n">
-        <v>1000000000</v>
+        <v>352170015</v>
       </c>
       <c r="G86" t="n">
-        <v>355615305.9848892</v>
+        <v>325884991.0735922</v>
       </c>
       <c r="H86" t="n">
-        <v>245871.7278312281</v>
+        <v>2089846.094569357</v>
       </c>
       <c r="I86" t="n">
-        <v>0.6350273196421226</v>
+        <v>0.9908478031301908</v>
       </c>
       <c r="J86" t="n">
-        <v>-6.643196769182858</v>
+        <v>-4.644378234338887</v>
       </c>
       <c r="K86" t="n">
-        <v>0.6852396906158676</v>
+        <v>1.020660640068891</v>
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xb62132e35a6c13ee1ee0f84dc5d40bad8d815206</t>
+          <t>https://etherscan.io/token/0x50d1c9771902476076ecfc8b2a83ad6b9355a4c9</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>enjin-coin</t>
+          <t>singularitynet</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -4336,45 +4340,45 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>ENJ</t>
+          <t>AGIX</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Enjin Coin</t>
+          <t>SingularityNET</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>1000000000</v>
+        <v>1215068775.262011</v>
       </c>
       <c r="F87" t="n">
-        <v>1000000000</v>
+        <v>2000000000</v>
       </c>
       <c r="G87" t="n">
-        <v>349307414.7309649</v>
+        <v>325512029.5458177</v>
       </c>
       <c r="H87" t="n">
-        <v>3220132.663927915</v>
+        <v>4325780.905022426</v>
       </c>
       <c r="I87" t="n">
-        <v>0.3493074147309649</v>
+        <v>0.2678959711359764</v>
       </c>
       <c r="J87" t="n">
-        <v>-0.7163738151696919</v>
+        <v>-5.44856891715</v>
       </c>
       <c r="K87" t="n">
-        <v>0.346768060592153</v>
+        <v>0.2782444885424071</v>
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xf629cbd94d3791c9250152bd8dfbdf380e2a3b9c</t>
+          <t>https://etherscan.io/token/0x8eb24319393716668d768dcec29356ae9cffe285</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>dydx</t>
+          <t>basic-attention-token</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -4382,41 +4386,45 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>DYDX</t>
+          <t>BAT</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>dYdX</t>
+          <t>Basic Attention Token</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>156256174</v>
+        <v>1489138514.416335</v>
       </c>
       <c r="F88" t="n">
-        <v>1000000000</v>
+        <v>1500000000</v>
       </c>
       <c r="G88" t="n">
-        <v>336681335.4683849</v>
+        <v>324550082.5066641</v>
       </c>
       <c r="H88" t="n">
-        <v>21154656.66639422</v>
+        <v>4751545.080582493</v>
       </c>
       <c r="I88" t="n">
-        <v>2.154675408015461</v>
+        <v>0.2179448582953822</v>
       </c>
       <c r="J88" t="n">
-        <v>-3.406606845095396</v>
+        <v>-1.216237185099306</v>
       </c>
       <c r="K88" t="n">
-        <v>2.166873080784029</v>
-      </c>
-      <c r="L88" t="inlineStr"/>
+        <v>0.2178898978875497</v>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>https://etherscan.io/token/Bat</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>basic-attention-token</t>
+          <t>dydx</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -4424,40 +4432,36 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>BAT</t>
+          <t>DYDX</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Basic Attention Token</t>
+          <t>dYdX</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>1489010445.416335</v>
+        <v>156256174</v>
       </c>
       <c r="F89" t="n">
-        <v>1500000000</v>
+        <v>1000000000</v>
       </c>
       <c r="G89" t="n">
-        <v>332790764.7402042</v>
+        <v>323471804.2254157</v>
       </c>
       <c r="H89" t="n">
-        <v>5294933.954522714</v>
+        <v>13875302.15763521</v>
       </c>
       <c r="I89" t="n">
-        <v>0.2234979383553983</v>
+        <v>2.070137748447724</v>
       </c>
       <c r="J89" t="n">
-        <v>-0.4457636093507535</v>
+        <v>-3.868077578344479</v>
       </c>
       <c r="K89" t="n">
-        <v>0.2232649032627045</v>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>https://etherscan.io/token/Bat</t>
-        </is>
-      </c>
+        <v>2.084871136985833</v>
+      </c>
+      <c r="L89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4479,23 +4483,23 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>816005425.4489994</v>
+        <v>816009222.0972039</v>
       </c>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="n">
-        <v>329683945.1447142</v>
+        <v>322389443.2264077</v>
       </c>
       <c r="H90" t="n">
-        <v>11054669.03928831</v>
+        <v>4259608.399352713</v>
       </c>
       <c r="I90" t="n">
-        <v>0.4040217563054911</v>
+        <v>0.3950806369538852</v>
       </c>
       <c r="J90" t="n">
-        <v>-2.180510951499239</v>
+        <v>-1.670272861484839</v>
       </c>
       <c r="K90" t="n">
-        <v>0.4034149683770319</v>
+        <v>0.3957557079784451</v>
       </c>
       <c r="L90" t="inlineStr">
         <is>
@@ -4506,7 +4510,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>singularitynet</t>
+          <t>oasis-network</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -4514,45 +4518,45 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>AGIX</t>
+          <t>ROSE</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>SingularityNET</t>
+          <t>Oasis Network</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>1215071357.26201</v>
+        <v>5725718533</v>
       </c>
       <c r="F91" t="n">
-        <v>2000000000</v>
+        <v>10000000000</v>
       </c>
       <c r="G91" t="n">
-        <v>322847016.6254143</v>
+        <v>295330877.6876655</v>
       </c>
       <c r="H91" t="n">
-        <v>2608379.387311816</v>
+        <v>4201813.752665015</v>
       </c>
       <c r="I91" t="n">
-        <v>0.265702104403896</v>
+        <v>0.0515797058457441</v>
       </c>
       <c r="J91" t="n">
-        <v>-0.1410275302433975</v>
+        <v>-2.275824319277888</v>
       </c>
       <c r="K91" t="n">
-        <v>0.2647682837134989</v>
+        <v>0.0518161390331874</v>
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x8eb24319393716668d768dcec29356ae9cffe285</t>
+          <t>https://www.oasisscan.com/</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>oasis-network</t>
+          <t>gnosis-gno</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -4560,45 +4564,45 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>ROSE</t>
+          <t>GNO</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Oasis Network</t>
+          <t>Gnosis</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>5725718533</v>
+        <v>2589588</v>
       </c>
       <c r="F92" t="n">
-        <v>10000000000</v>
+        <v>3000000</v>
       </c>
       <c r="G92" t="n">
-        <v>307443059.3641433</v>
+        <v>294894584.509603</v>
       </c>
       <c r="H92" t="n">
-        <v>6552270.028453106</v>
+        <v>655849.0383693228</v>
       </c>
       <c r="I92" t="n">
-        <v>0.0536951052679598</v>
+        <v>113.8770277393945</v>
       </c>
       <c r="J92" t="n">
-        <v>-1.392992860928722</v>
+        <v>-1.825494014528476</v>
       </c>
       <c r="K92" t="n">
-        <v>0.0535582538849285</v>
+        <v>114.7748091631518</v>
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>https://www.oasisscan.com/</t>
+          <t>https://etherscan.io/token/Gnosis</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>gnosis-gno</t>
+          <t>nem</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -4606,45 +4610,45 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>GNO</t>
+          <t>XEM</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Gnosis</t>
+          <t>NEM</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>2589588</v>
+        <v>8999999999</v>
       </c>
       <c r="F93" t="n">
-        <v>3000000</v>
+        <v>8999999999</v>
       </c>
       <c r="G93" t="n">
-        <v>297819980.4389846</v>
+        <v>288854685.9004815</v>
       </c>
       <c r="H93" t="n">
-        <v>1603745.081432911</v>
+        <v>4727842.393705336</v>
       </c>
       <c r="I93" t="n">
-        <v>115.0067039386128</v>
+        <v>0.0320949651036196</v>
       </c>
       <c r="J93" t="n">
-        <v>-1.592648193200076</v>
+        <v>-2.373843772515627</v>
       </c>
       <c r="K93" t="n">
-        <v>114.1757349454641</v>
+        <v>0.0323970781669824</v>
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/Gnosis</t>
+          <t>http://nembex.nem.ninja/</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>nem</t>
+          <t>holo</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -4652,45 +4656,43 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>XEM</t>
+          <t>HOT</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>NEM</t>
+          <t>Holo</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>8999999999</v>
-      </c>
-      <c r="F94" t="n">
-        <v>8999999999</v>
-      </c>
+        <v>173467411323.5712</v>
+      </c>
+      <c r="F94" t="inlineStr"/>
       <c r="G94" t="n">
-        <v>295791282.8353472</v>
+        <v>281779908.8413673</v>
       </c>
       <c r="H94" t="n">
-        <v>4908338.361317076</v>
+        <v>1008099.361328413</v>
       </c>
       <c r="I94" t="n">
-        <v>0.0328656980964681</v>
+        <v>0.0016243968056672</v>
       </c>
       <c r="J94" t="n">
-        <v>-1.020519136284316</v>
+        <v>-2.746172917173</v>
       </c>
       <c r="K94" t="n">
-        <v>0.0329346488106602</v>
+        <v>0.0016365268667484</v>
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>http://nembex.nem.ninja/</t>
+          <t>https://etherscan.io/token/0x6c6ee5e31d828de241282b9606c8e98ea48526e2</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>holo</t>
+          <t>ravencoin</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -4698,36 +4700,38 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>HOT</t>
+          <t>RVN</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Holo</t>
+          <t>Ravencoin</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>173467411323.5712</v>
-      </c>
-      <c r="F95" t="inlineStr"/>
+        <v>12557072325.67762</v>
+      </c>
+      <c r="F95" t="n">
+        <v>21000000000</v>
+      </c>
       <c r="G95" t="n">
-        <v>292636037.5546633</v>
+        <v>271263713.6561846</v>
       </c>
       <c r="H95" t="n">
-        <v>1417516.820584966</v>
+        <v>2212350.86846921</v>
       </c>
       <c r="I95" t="n">
-        <v>0.0016869799077638</v>
+        <v>0.0216024648597018</v>
       </c>
       <c r="J95" t="n">
-        <v>-0.940985110254564</v>
+        <v>-1.680707502753993</v>
       </c>
       <c r="K95" t="n">
-        <v>0.0016810897797844</v>
+        <v>0.0217602042491664</v>
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0x6c6ee5e31d828de241282b9606c8e98ea48526e2</t>
+          <t>https://ravencoin.network/</t>
         </is>
       </c>
     </row>
@@ -4751,25 +4755,25 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>104662242</v>
+        <v>104666069.5</v>
       </c>
       <c r="F96" t="n">
         <v>107822406</v>
       </c>
       <c r="G96" t="n">
-        <v>277599150.8338653</v>
+        <v>268445937.8843515</v>
       </c>
       <c r="H96" t="n">
-        <v>6188522.676846213</v>
+        <v>5249772.222795</v>
       </c>
       <c r="I96" t="n">
-        <v>2.652333310745105</v>
+        <v>2.56478474033413</v>
       </c>
       <c r="J96" t="n">
-        <v>-0.4610852739219208</v>
+        <v>-2.352743427762091</v>
       </c>
       <c r="K96" t="n">
-        <v>2.63350501126252</v>
+        <v>2.578817245018877</v>
       </c>
       <c r="L96" t="inlineStr">
         <is>
@@ -4780,7 +4784,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>ravencoin</t>
+          <t>balancer</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -4788,45 +4792,45 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>RVN</t>
+          <t>BAL</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Ravencoin</t>
+          <t>Balancer</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>12546898910.67762</v>
+        <v>49572909.80123565</v>
       </c>
       <c r="F97" t="n">
-        <v>21000000000</v>
+        <v>96150704</v>
       </c>
       <c r="G97" t="n">
-        <v>272872209.5212311</v>
+        <v>263490937.9938633</v>
       </c>
       <c r="H97" t="n">
-        <v>2598182.339263153</v>
+        <v>980083.6936695456</v>
       </c>
       <c r="I97" t="n">
-        <v>0.0217481794875236</v>
+        <v>5.315220330021773</v>
       </c>
       <c r="J97" t="n">
-        <v>-2.539359895583207</v>
+        <v>-1.09011515684507</v>
       </c>
       <c r="K97" t="n">
-        <v>0.0218910624010586</v>
+        <v>5.336747881182022</v>
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>https://ravencoin.network/</t>
+          <t>https://etherscan.io/token/0xba100000625a3754423978a60c9317c58a424e3D</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>balancer</t>
+          <t>theta-fuel</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -4834,45 +4838,43 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>BAL</t>
+          <t>TFUEL</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Balancer</t>
+          <t>Theta Fuel</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>49536028.68303556</v>
-      </c>
-      <c r="F98" t="n">
-        <v>96150704</v>
-      </c>
+        <v>6144767310</v>
+      </c>
+      <c r="F98" t="inlineStr"/>
       <c r="G98" t="n">
-        <v>271891989.4924653</v>
+        <v>257885655.672425</v>
       </c>
       <c r="H98" t="n">
-        <v>1117061.226627232</v>
+        <v>711876.0877765957</v>
       </c>
       <c r="I98" t="n">
-        <v>5.488772449487443</v>
+        <v>0.0419683354409111</v>
       </c>
       <c r="J98" t="n">
-        <v>-1.042600473968966</v>
+        <v>-3.76252749884678</v>
       </c>
       <c r="K98" t="n">
-        <v>5.509396466329249</v>
+        <v>0.0426316523430807</v>
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xba100000625a3754423978a60c9317c58a424e3D</t>
+          <t>https://explorer.thetatoken.org/</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>theta-fuel</t>
+          <t>compound</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -4880,43 +4882,45 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>TFUEL</t>
+          <t>COMP</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Theta Fuel</t>
+          <t>Compound</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>6141405684</v>
-      </c>
-      <c r="F99" t="inlineStr"/>
+        <v>7460510.277832701</v>
+      </c>
+      <c r="F99" t="n">
+        <v>10000000</v>
+      </c>
       <c r="G99" t="n">
-        <v>271063073.1044181</v>
+        <v>257527143.1614802</v>
       </c>
       <c r="H99" t="n">
-        <v>737862.768239761</v>
+        <v>2727037.610054137</v>
       </c>
       <c r="I99" t="n">
-        <v>0.0441369756455936</v>
+        <v>34.51870362362031</v>
       </c>
       <c r="J99" t="n">
-        <v>-1.538442991931061</v>
+        <v>-2.774067431032237</v>
       </c>
       <c r="K99" t="n">
-        <v>0.044285181655338</v>
+        <v>34.76259293032071</v>
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>https://explorer.thetatoken.org/</t>
+          <t>https://etherscan.io/token/0xc00e94cb662c3520282e6f5717214004a7f26888</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>compound</t>
+          <t>celo</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -4924,45 +4928,45 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>COMP</t>
+          <t>CELO</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Compound</t>
+          <t>Celo</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>7459320.799104461</v>
+        <v>498369748</v>
       </c>
       <c r="F100" t="n">
-        <v>10000000</v>
+        <v>1000000000</v>
       </c>
       <c r="G100" t="n">
-        <v>266504457.6748421</v>
+        <v>255606366.9385819</v>
       </c>
       <c r="H100" t="n">
-        <v>4638482.131763434</v>
+        <v>1023444.398006444</v>
       </c>
       <c r="I100" t="n">
-        <v>35.7277109876864</v>
+        <v>0.5128849974629317</v>
       </c>
       <c r="J100" t="n">
-        <v>-0.8046232331897245</v>
+        <v>-2.879481960842137</v>
       </c>
       <c r="K100" t="n">
-        <v>35.66626885000192</v>
+        <v>0.5181104206781993</v>
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>https://etherscan.io/token/0xc00e94cb662c3520282e6f5717214004a7f26888</t>
+          <t>https://explorer.celo.org/blocks</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>celo</t>
+          <t>audius</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -4970,38 +4974,36 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>CELO</t>
+          <t>AUDIO</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Celo</t>
+          <t>Audius</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>498369748</v>
-      </c>
-      <c r="F101" t="n">
-        <v>1000000000</v>
-      </c>
+        <v>1045289093</v>
+      </c>
+      <c r="F101" t="inlineStr"/>
       <c r="G101" t="n">
-        <v>263672831.175586</v>
+        <v>255176237.2545941</v>
       </c>
       <c r="H101" t="n">
-        <v>1387460.744640871</v>
+        <v>2056227.161254124</v>
       </c>
       <c r="I101" t="n">
-        <v>0.5290706994831196</v>
+        <v>0.2441202524387137</v>
       </c>
       <c r="J101" t="n">
-        <v>-3.451535927916565</v>
+        <v>-0.2256495672171907</v>
       </c>
       <c r="K101" t="n">
-        <v>0.534993471155054</v>
+        <v>0.239491232449818</v>
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>https://explorer.celo.org/blocks</t>
+          <t>https://etherscan.io/token/0x18aaa7115705e8be94bffebde57af9bfc265b998</t>
         </is>
       </c>
     </row>

</xml_diff>